<commit_message>
Solicitudes OAI Julio 2023
</commit_message>
<xml_diff>
--- a/Estadísticas Solicitudes OAI, CNCCDL, 2019-2022.xlsx
+++ b/Estadísticas Solicitudes OAI, CNCCDL, 2019-2022.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jp.demola\Documents\MEGA\MEGAsync\datosabiertos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jp.demola\Documents\MEGA\MEGAsync\datosabiertos\Datos Abiertos CNCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4E346812-5307-4DA8-A90E-9445A6A30504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B090FB23-E7C4-4C56-AED5-18C41ECB317C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="88">
   <si>
     <t>Fecha_Solicitud</t>
   </si>
@@ -172,113 +172,122 @@
   </si>
   <si>
     <t>10/27/2020</t>
-  </si>
-  <si>
-    <t>10/21/2019</t>
-  </si>
-  <si>
-    <t>información sobre el procedimiento que ha de realizar una empresa privada si quiere conseguir los Certificados de Emisiones Reducidas (CERs)</t>
-  </si>
-  <si>
-    <t>10/20/2020</t>
-  </si>
-  <si>
-    <t>NECESITO UN JUEGO COMPLETO DE LOS ORIGINALES</t>
-  </si>
-  <si>
-    <t>NECESITO LA COPIA CERTIFICADA</t>
-  </si>
-  <si>
-    <t>COPIA CERTIFICADA</t>
-  </si>
-  <si>
-    <t>1/28/2019</t>
-  </si>
-  <si>
-    <t>Solicitud información sobre cantidad de servidores con que cuenta la institución.</t>
-  </si>
-  <si>
-    <t>1/22/2019</t>
-  </si>
-  <si>
-    <t>Solicitud información sobre Presupuesto Institcucional.</t>
-  </si>
-  <si>
-    <t>1/17/2019</t>
-  </si>
-  <si>
-    <t>Solicitud información sobre los diferentes Proyectos que desarrolla el CNCCMDL.</t>
-  </si>
-  <si>
-    <t>07/21/2020</t>
-  </si>
-  <si>
-    <t>Estadísticas generadas con relación a los avances en temas de cambio climático en el país, así cómo la base de datos de organizaciones y asociaciones que trabajan los temas ambientales o cambio climático en el país. Muchas gracias anticipadas.</t>
-  </si>
-  <si>
-    <t>06/23/2020</t>
-  </si>
-  <si>
-    <t>Factor de emisiones del SENI (t CO2/MWh)</t>
-  </si>
-  <si>
-    <t>01/19/2020</t>
-  </si>
-  <si>
-    <t>Información sobre sistema de clasificación de la basura</t>
-  </si>
-  <si>
-    <t>Buenas tardes, estoy interesada en la metodologia para el calculo de la huella de carbono y emisiones de CO2 de la Republica Dominicana utilizada en el documento de la contribucion nacional determinada.  O si poseen algun otro tipo de documento relacionado al calculo de la huella de carbono,calculo de emisiones del transporte, etc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Necesito conocer el factor de emisión 2020 ó 2021 en el sector de energía Rep. Dominicana. Un catedrático español me indicó podía conocer el factor de emisión a través de la distribuidora de energía (Edeeste, en este caso) que suple a la organización de interés. Sin embargo, Edeeste me informó no maneja la información de factores de emisión porque no son generadores de energía. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proyecto Completo implementado o en implementación  en Rep. Dominicana sobre Mecanismo de Desarrollo Limpio y Mercado de Carbono. Todos los pasos o procesos requeridos. </t>
-  </si>
-  <si>
-    <t>Que mecanismos se estan implementando a nivel nacional para mitigar los efectos del cambio climatico, producidos en consecuencia del uso de fuentes NO renovables de energia.</t>
-  </si>
-  <si>
-    <t>1.Producción local de desechos plásticos 2.Generacion de desechos plásticos por tipo y provincia 3.Volumen de residuos solidos en RD por vertedero 4.Costo de producción y materia prima</t>
-  </si>
-  <si>
-    <t>Solicito información relacionada al cambio climático, ya sean, proyectos, investigaciones y otros, desarrollados en el Municipio Villa La Mata, Provincia Sánchez Ramírez , los mismos me servirán de apoyo a la investigación.</t>
-  </si>
-  <si>
-    <t>Favor confirmar si actualmente están disponibles los créditos de mecanismo de desarrollo limpio, en caso de que estén  ¿Cuál es el proceso para someter un Proyecto de Mecanismo de Desarrollo Limpio?; y ¿Qué tipo de iniciativas pueden aplicar a estos créditos?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Política turística en referencia al desarrollo sostenible de la hostelería (gestión del territorio, uso y gestión de residuos) - Cantidad de establecimientos hoteleros fuera del ámbito de sol y playa, por ejemplo: turismo cultural o rural - Número de turistas en búsqueda de otra tipología de vacaciones que no sea sol y playa  - Impacto medioambiental del turismo en la isla  - Proyección futura referente al cambio climático y gestión medioambiental del país </t>
-  </si>
-  <si>
-    <t>Medidas y Resoñuciones adoptadas como politicas publicas para mitigar los efectos del cambio climatico en RD y afianzar el pais en el campo internacional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">investigación sobre la sostenibilidad ambiental del país </t>
-  </si>
-  <si>
-    <t xml:space="preserve">¿Cómo está el estatus del acuerdo de país? ¿Se aplica en nuestro país dicho acuerdo, y de qué modo se aplica? Información de eficiencia energética en nuestro país y su impacto favorable con el medioambiente. Nivel o índice de riesgo climático del país. </t>
-  </si>
-  <si>
-    <t>CONOCER LA CARTA COMPROMISO AL CIUDADANO</t>
-  </si>
-  <si>
-    <t>Estudios completos sobre las vulnerabilidades de las zonas costeros-marinas en la República Dominicana y cualquier otro estudio que hayan realizado y tenga que ver con el medio ambiente marino.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Han cogido préstamos en los últimos 3 años?  2. Cuál es la composición de esos préstamos?  3. Cuál es el monto actual de deuda a corto, mediano y largo plazo?  4. A qué organismos de intermediación financiera y no financiera han cogido préstamos?  5. Cuál es el origen de los fondos adeudados?  6. Cuál es el porcentaje de libramiento adeudado aplicado al gasto público de su institución?  7. Qué estrategia tienen para aplicar los fondos públicos a la porción corriente de la deuda a largo plazo y del gasto nominal? </t>
-  </si>
-  <si>
-    <t>Nómina</t>
-  </si>
-  <si>
-    <t>Medidas generales implementadas por el estado dominicano para mitigar el cambio climático 2019-2021</t>
   </si>
   <si>
     <t>Buenas, Me interesaría obtener información sobre los planes que se están llevando a acabo para cumplir con el objetivo numero 11: Ciudades y comunidades sostenibles, mas específicamente sobre el indicador numero 11.6.1 : "Proporción de residuos sólidos urbanos recolectados regularmente y con descarga final adecuada del total de residuos sólidos urbanos generados, desglosada por ciudad".
 Dentro de los archivos me gustaría recibir los planes a corto y largo plazo que se están aplicando y los resultados hasta el momento y proyecciones futuras (si es posible incluir gráficos ).
 En caso de poder acceder a mas información online de manera directa, les agradecería de sobremanera si me facilitaran los links.</t>
+  </si>
+  <si>
+    <t>10/21/2019</t>
+  </si>
+  <si>
+    <t>información sobre el procedimiento que ha de realizar una empresa privada si quiere conseguir los Certificados de Emisiones Reducidas (CERs)</t>
+  </si>
+  <si>
+    <t>10/20/2020</t>
+  </si>
+  <si>
+    <t>NECESITO UN JUEGO COMPLETO DE LOS ORIGINALES</t>
+  </si>
+  <si>
+    <t>NECESITO LA COPIA CERTIFICADA</t>
+  </si>
+  <si>
+    <t>COPIA CERTIFICADA</t>
+  </si>
+  <si>
+    <t>1/28/2019</t>
+  </si>
+  <si>
+    <t>Solicitud información sobre cantidad de servidores con que cuenta la institución.</t>
+  </si>
+  <si>
+    <t>1/22/2019</t>
+  </si>
+  <si>
+    <t>Solicitud información sobre Presupuesto Institcucional.</t>
+  </si>
+  <si>
+    <t>1/17/2019</t>
+  </si>
+  <si>
+    <t>Solicitud información sobre los diferentes Proyectos que desarrolla el CNCCMDL.</t>
+  </si>
+  <si>
+    <t>07/21/2020</t>
+  </si>
+  <si>
+    <t>Estadísticas generadas con relación a los avances en temas de cambio climático en el país, así cómo la base de datos de organizaciones y asociaciones que trabajan los temas ambientales o cambio climático en el país. Muchas gracias anticipadas.</t>
+  </si>
+  <si>
+    <t>06/23/2020</t>
+  </si>
+  <si>
+    <t>Factor de emisiones del SENI (t CO2/MWh)</t>
+  </si>
+  <si>
+    <t>01/19/2020</t>
+  </si>
+  <si>
+    <t>Información sobre sistema de clasificación de la basura</t>
+  </si>
+  <si>
+    <t>Buenas tardes, estoy interesada en la metodologia para el calculo de la huella de carbono y emisiones de CO2 de la Republica Dominicana utilizada en el documento de la contribucion nacional determinada.  O si poseen algun otro tipo de documento relacionado al calculo de la huella de carbono,calculo de emisiones del transporte, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Necesito conocer el factor de emisión 2020 ó 2021 en el sector de energía Rep. Dominicana. Un catedrático español me indicó podía conocer el factor de emisión a través de la distribuidora de energía (Edeeste, en este caso) que suple a la organización de interés. Sin embargo, Edeeste me informó no maneja la información de factores de emisión porque no son generadores de energía. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proyecto Completo implementado o en implementación  en Rep. Dominicana sobre Mecanismo de Desarrollo Limpio y Mercado de Carbono. Todos los pasos o procesos requeridos. </t>
+  </si>
+  <si>
+    <t>Que mecanismos se estan implementando a nivel nacional para mitigar los efectos del cambio climatico, producidos en consecuencia del uso de fuentes NO renovables de energia.</t>
+  </si>
+  <si>
+    <t>1.Producción local de desechos plásticos 2.Generacion de desechos plásticos por tipo y provincia 3.Volumen de residuos solidos en RD por vertedero 4.Costo de producción y materia prima</t>
+  </si>
+  <si>
+    <t>Solicito información relacionada al cambio climático, ya sean, proyectos, investigaciones y otros, desarrollados en el Municipio Villa La Mata, Provincia Sánchez Ramírez , los mismos me servirán de apoyo a la investigación.</t>
+  </si>
+  <si>
+    <t>Favor confirmar si actualmente están disponibles los créditos de mecanismo de desarrollo limpio, en caso de que estén  ¿Cuál es el proceso para someter un Proyecto de Mecanismo de Desarrollo Limpio?; y ¿Qué tipo de iniciativas pueden aplicar a estos créditos?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Política turística en referencia al desarrollo sostenible de la hostelería (gestión del territorio, uso y gestión de residuos) - Cantidad de establecimientos hoteleros fuera del ámbito de sol y playa, por ejemplo: turismo cultural o rural - Número de turistas en búsqueda de otra tipología de vacaciones que no sea sol y playa  - Impacto medioambiental del turismo en la isla  - Proyección futura referente al cambio climático y gestión medioambiental del país </t>
+  </si>
+  <si>
+    <t>Medidas y Resoñuciones adoptadas como politicas publicas para mitigar los efectos del cambio climatico en RD y afianzar el pais en el campo internacional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">investigación sobre la sostenibilidad ambiental del país </t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Cómo está el estatus del acuerdo de país? ¿Se aplica en nuestro país dicho acuerdo, y de qué modo se aplica? Información de eficiencia energética en nuestro país y su impacto favorable con el medioambiente. Nivel o índice de riesgo climático del país. </t>
+  </si>
+  <si>
+    <t>CONOCER LA CARTA COMPROMISO AL CIUDADANO</t>
+  </si>
+  <si>
+    <t>Estudios completos sobre las vulnerabilidades de las zonas costeros-marinas en la República Dominicana y cualquier otro estudio que hayan realizado y tenga que ver con el medio ambiente marino.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Han cogido préstamos en los últimos 3 años?  2. Cuál es la composición de esos préstamos?  3. Cuál es el monto actual de deuda a corto, mediano y largo plazo?  4. A qué organismos de intermediación financiera y no financiera han cogido préstamos?  5. Cuál es el origen de los fondos adeudados?  6. Cuál es el porcentaje de libramiento adeudado aplicado al gasto público de su institución?  7. Qué estrategia tienen para aplicar los fondos públicos a la porción corriente de la deuda a largo plazo y del gasto nominal? </t>
+  </si>
+  <si>
+    <t>Nómina</t>
+  </si>
+  <si>
+    <t>Medidas generales implementadas por el estado dominicano para mitigar el cambio climático 2019-2021</t>
+  </si>
+  <si>
+    <t>Reportes, informes, estadísticas y/o estudios más recientes sobre medidas de adaptación al cambio climático en general a nivel nacional y local</t>
+  </si>
+  <si>
+    <t>convenios internacionales en materia DE MITIGACION Y adaptacion al cambio climatico , asumidos por período 2019-2021.</t>
+  </si>
+  <si>
+    <t>21 dias</t>
   </si>
 </sst>
 </file>
@@ -762,9 +771,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1120,13 +1132,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1258,7 +1274,7 @@
       <c r="A10" s="1">
         <v>43642</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C10" t="s">
@@ -1342,7 +1358,7 @@
       <c r="A16" s="1">
         <v>43560</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C16" t="s">
@@ -1619,7 +1635,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>46</v>
       </c>
       <c r="B36" t="s">
@@ -1647,11 +1663,11 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>49</v>
       </c>
-      <c r="B38" t="s">
-        <v>84</v>
+      <c r="B38" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
@@ -1661,11 +1677,11 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>50</v>
+      <c r="A39" t="s">
+        <v>51</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
@@ -1675,11 +1691,11 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>52</v>
+      <c r="A40" t="s">
+        <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -1693,7 +1709,7 @@
         <v>44175</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -1707,7 +1723,7 @@
         <v>44114</v>
       </c>
       <c r="B42" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
@@ -1717,11 +1733,11 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>56</v>
+      <c r="A43" t="s">
+        <v>57</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>
@@ -1731,11 +1747,11 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>58</v>
+      <c r="A44" t="s">
+        <v>59</v>
       </c>
       <c r="B44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
@@ -1745,11 +1761,11 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>60</v>
+      <c r="A45" t="s">
+        <v>61</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -1759,11 +1775,11 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>62</v>
+      <c r="A46" t="s">
+        <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
@@ -1773,11 +1789,11 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>64</v>
+      <c r="A47" t="s">
+        <v>65</v>
       </c>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
@@ -1787,11 +1803,11 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>66</v>
+      <c r="A48" t="s">
+        <v>67</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
@@ -1805,7 +1821,7 @@
         <v>44235</v>
       </c>
       <c r="B49" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
@@ -1819,7 +1835,7 @@
         <v>44328</v>
       </c>
       <c r="B50" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
@@ -1833,7 +1849,7 @@
         <v>44344</v>
       </c>
       <c r="B51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
@@ -1847,7 +1863,7 @@
         <v>44350</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
@@ -1861,7 +1877,7 @@
         <v>44363</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
@@ -1875,7 +1891,7 @@
         <v>44398</v>
       </c>
       <c r="B54" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C54" t="s">
         <v>5</v>
@@ -1889,7 +1905,7 @@
         <v>44480</v>
       </c>
       <c r="B55" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
@@ -1903,7 +1919,7 @@
         <v>44503</v>
       </c>
       <c r="B56" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
@@ -1917,7 +1933,7 @@
         <v>44634</v>
       </c>
       <c r="B57" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
@@ -1931,7 +1947,7 @@
         <v>44670</v>
       </c>
       <c r="B58" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
@@ -1945,7 +1961,7 @@
         <v>44705</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
@@ -1959,7 +1975,7 @@
         <v>44736</v>
       </c>
       <c r="B60" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
@@ -1973,7 +1989,7 @@
         <v>44778</v>
       </c>
       <c r="B61" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
@@ -1987,7 +2003,7 @@
         <v>44793</v>
       </c>
       <c r="B62" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -2001,7 +2017,7 @@
         <v>45013</v>
       </c>
       <c r="B63" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C63" t="s">
         <v>5</v>
@@ -2015,17 +2031,44 @@
         <v>45071</v>
       </c>
       <c r="B64" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
       </c>
       <c r="D64">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>45091</v>
+      </c>
+      <c r="B65" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" t="s">
+        <v>87</v>
+      </c>
+      <c r="D65">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>45099</v>
+      </c>
+      <c r="B66" t="s">
+        <v>86</v>
+      </c>
+      <c r="C66" t="s">
+        <v>87</v>
+      </c>
+      <c r="D66">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>